<commit_message>
change dashboard name dynamically
</commit_message>
<xml_diff>
--- a/report_logs.xlsx
+++ b/report_logs.xlsx
@@ -16,10 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="3">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,7 +28,6 @@
     <font>
       <b val="1"/>
     </font>
-    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -46,7 +43,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -54,20 +51,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="date_format" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -430,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,149 +483,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>IT65329330</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Sangay</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>12190015.gcit@rub.edu.bt</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>45078.8687143834</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">done
-</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>estate</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>45078.91689578184</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>IT65329330</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Sangay</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>12190015.gcit@rub.edu.bt</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>45078.91768421146</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>done</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>estate</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>45078.92578993255</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>IT65329330</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Sangay</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>12190015.gcit@rub.edu.bt</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45078.92708391199</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>estate</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>45078.92718397716</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>IT65329330</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Sangay</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>12190015.gcit@rub.edu.bt</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>45078.92740149055</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>estate</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>45078.93072955289</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>